<commit_message>
Outcomes using actual tournament teams
This outcomes file uses an adjusted model that includes the teams that qualified for the tournament as selected by the selection committee or by an automatic bid. Calculations within the model remained unchanged.
</commit_message>
<xml_diff>
--- a/actualTourneyTeamsOutcomes.xlsx
+++ b/actualTourneyTeamsOutcomes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isaiahnick/Desktop/NCAAM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6BBD18C-D5A8-2645-95ED-368EF3B80307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55CB4E0A-CBFF-A24D-AEED-1B5FFD71D066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="28700" windowHeight="19940" xr2:uid="{48E97E4C-EE8F-4D4C-B07B-683BDA3BBCA7}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="28700" windowHeight="19940" activeTab="3" xr2:uid="{48E97E4C-EE8F-4D4C-B07B-683BDA3BBCA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Champions" sheetId="2" r:id="rId1"/>
@@ -512,9 +512,6 @@
     <t>UC San Diego</t>
   </si>
   <si>
-    <t>Number of teams meeting criteria: 44</t>
-  </si>
-  <si>
     <t>Xavier</t>
   </si>
   <si>
@@ -576,6 +573,9 @@
   </si>
   <si>
     <t>Number of teams meeting criteria: 39</t>
+  </si>
+  <si>
+    <t>Number of teams meeting criteria: 46</t>
   </si>
 </sst>
 </file>
@@ -963,7 +963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18BC26E8-D6C2-0E4A-830A-7AA78E1502E8}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -1005,7 +1005,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -1398,7 +1398,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -1897,7 +1897,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -2719,7 +2719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0825CF93-4158-144F-A7C0-50341FAA3534}">
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
@@ -2761,7 +2761,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -3806,7 +3806,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -4784,7 +4784,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B48" t="s">
         <v>46</v>
@@ -4810,7 +4810,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B49" t="s">
         <v>25</v>
@@ -4895,7 +4895,7 @@
   <dimension ref="A1:H63"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4935,7 +4935,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>156</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -5959,7 +5959,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B50" t="s">
         <v>4</v>
@@ -5985,7 +5985,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B51" t="s">
         <v>46</v>
@@ -6063,7 +6063,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B54" t="s">
         <v>25</v>
@@ -6089,7 +6089,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B55" t="s">
         <v>4</v>
@@ -6314,7 +6314,7 @@
         <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C11">
         <v>17.3</v>
@@ -6347,7 +6347,7 @@
         <v>126</v>
       </c>
       <c r="B14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C14">
         <v>13.69</v>
@@ -6413,7 +6413,7 @@
         <v>121</v>
       </c>
       <c r="B20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C20">
         <v>6.88</v>
@@ -6446,7 +6446,7 @@
         <v>124</v>
       </c>
       <c r="B23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C23">
         <v>4.16</v>
@@ -6457,7 +6457,7 @@
         <v>131</v>
       </c>
       <c r="B24" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C24">
         <v>2.08</v>
@@ -6479,7 +6479,7 @@
         <v>126</v>
       </c>
       <c r="B26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C26">
         <v>0.51</v>
@@ -6490,7 +6490,7 @@
         <v>128</v>
       </c>
       <c r="B27" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C27">
         <v>0.39</v>
@@ -6512,7 +6512,7 @@
         <v>125</v>
       </c>
       <c r="B29" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C29">
         <v>-4.3099999999999996</v>
@@ -6523,7 +6523,7 @@
         <v>136</v>
       </c>
       <c r="B30" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C30">
         <v>-5.98</v>
@@ -6534,7 +6534,7 @@
         <v>134</v>
       </c>
       <c r="B31" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C31">
         <v>-6.67</v>
@@ -6545,7 +6545,7 @@
         <v>135</v>
       </c>
       <c r="B32" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C32">
         <v>-9.23</v>
@@ -6556,7 +6556,7 @@
         <v>133</v>
       </c>
       <c r="B33" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C33">
         <v>-12.76</v>
@@ -6913,7 +6913,7 @@
         <v>4</v>
       </c>
       <c r="B67" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C67">
         <v>17.690000000000001</v>
@@ -6935,7 +6935,7 @@
         <v>25</v>
       </c>
       <c r="B69" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C69">
         <v>17.170000000000002</v>
@@ -6968,7 +6968,7 @@
         <v>4</v>
       </c>
       <c r="B72" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C72">
         <v>16.16</v>
@@ -6979,7 +6979,7 @@
         <v>46</v>
       </c>
       <c r="B73" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C73">
         <v>15.23</v>

</xml_diff>